<commit_message>
Atualiza código do painel
</commit_message>
<xml_diff>
--- a/Casos dengue - Fortaleza - 2022.xlsx
+++ b/Casos dengue - Fortaleza - 2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge\OneDrive\Desktop\Denguefortaleza\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD35E991-DD24-4FC7-BEE3-1B2E1E120517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56911B1A-C22B-4F6B-BEC9-C2A6A6D861C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{32B877CD-17A9-4514-806C-D495F1B6667D}"/>
   </bookViews>
@@ -390,9 +390,6 @@
     <t>OLAVO OLIVEIRA</t>
   </si>
   <si>
-    <t>DENGUE TOTAL</t>
-  </si>
-  <si>
     <t>CASOS GRAVES TOTAIS</t>
   </si>
   <si>
@@ -409,6 +406,9 @@
   </si>
   <si>
     <t>DENGUE: CLASSIFICAÇÃO,TAXA DE INCIDÊNCIA E LETALIDADE POR bairro DE RESIDÊNCIA, FORTALEZA 2022</t>
+  </si>
+  <si>
+    <t>CASOS DE DENGUE TOTAIS</t>
   </si>
 </sst>
 </file>
@@ -1385,8 +1385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB68A67-CB3D-4F4A-A3CD-34EEED385B20}">
   <dimension ref="A1:J130"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1404,7 +1404,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -1421,25 +1421,25 @@
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="E5" s="13" t="s">
+      <c r="F5" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="G5" s="10" t="s">
         <v>120</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>